<commit_message>
Update SQL data dictionary and sync package files to origin/main
</commit_message>
<xml_diff>
--- a/Documentation/Data_Dictionary(Bike-Rental DBMS).xlsx
+++ b/Documentation/Data_Dictionary(Bike-Rental DBMS).xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEA10FD-0165-4ADD-A67C-D4C80E055771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861C1E7D-1C83-451F-8214-940AEB64E914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,6 +27,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -485,7 +488,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2477,11 +2480,11 @@
   </sheetPr>
   <dimension ref="B6:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
@@ -2491,7 +2494,7 @@
     <col min="6" max="6" width="98.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
@@ -2508,7 +2511,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
@@ -2525,7 +2528,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
@@ -2572,7 +2575,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>26</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
@@ -2604,7 +2607,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
@@ -2619,7 +2622,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>29</v>
       </c>
@@ -2634,7 +2637,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>140</v>
       </c>
@@ -2649,12 +2652,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="15.75">
+    <row r="19" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>17</v>
       </c>
@@ -2671,7 +2674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
         <v>47</v>
       </c>
@@ -2688,7 +2691,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>22</v>
       </c>
@@ -2705,7 +2708,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>48</v>
       </c>
@@ -2722,7 +2725,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>49</v>
       </c>
@@ -2737,7 +2740,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
         <v>50</v>
       </c>
@@ -2752,7 +2755,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
         <v>141</v>
       </c>
@@ -2769,7 +2772,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
         <v>143</v>
       </c>
@@ -2786,7 +2789,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
         <v>51</v>
       </c>
@@ -2801,7 +2804,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
         <v>129</v>
       </c>
@@ -2816,7 +2819,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>147</v>
       </c>
@@ -2831,12 +2834,12 @@
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="15.75">
+    <row r="35" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>17</v>
       </c>
@@ -2853,7 +2856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
         <v>48</v>
       </c>
@@ -2870,7 +2873,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
         <v>56</v>
       </c>
@@ -2887,7 +2890,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>57</v>
       </c>
@@ -2902,7 +2905,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
         <v>58</v>
       </c>
@@ -2917,7 +2920,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
         <v>59</v>
       </c>
@@ -2932,7 +2935,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="2:6">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="9" t="s">
         <v>64</v>
       </c>
@@ -2947,7 +2950,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="9" t="s">
         <v>60</v>
       </c>
@@ -2962,7 +2965,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
         <v>61</v>
       </c>
@@ -2979,12 +2982,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="15.75">
+    <row r="49" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="2:6">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>17</v>
       </c>
@@ -3001,7 +3004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="2:6">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>66</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="2:6">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
         <v>67</v>
       </c>
@@ -3035,7 +3038,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="2:6">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="9" t="s">
         <v>24</v>
       </c>
@@ -3050,7 +3053,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
         <v>25</v>
       </c>
@@ -3065,7 +3068,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="2:6">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>68</v>
       </c>
@@ -3082,7 +3085,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
         <v>27</v>
       </c>
@@ -3097,7 +3100,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="2:6">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
         <v>69</v>
       </c>
@@ -3112,7 +3115,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
         <v>70</v>
       </c>
@@ -3127,7 +3130,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="9" t="s">
         <v>61</v>
       </c>
@@ -3142,12 +3145,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="15.75">
+    <row r="62" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="2:6">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="8" t="s">
         <v>17</v>
       </c>
@@ -3164,7 +3167,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="2:6">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="9" t="s">
         <v>80</v>
       </c>
@@ -3181,7 +3184,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="2:6">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="10" t="s">
         <v>47</v>
       </c>
@@ -3198,7 +3201,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="2:6">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="9" t="s">
         <v>81</v>
       </c>
@@ -3213,7 +3216,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="2:6">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="10" t="s">
         <v>82</v>
       </c>
@@ -3228,7 +3231,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="2:6">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="9" t="s">
         <v>83</v>
       </c>
@@ -3243,7 +3246,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="2:6">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="9" t="s">
         <v>84</v>
       </c>
@@ -3260,12 +3263,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="2:6" ht="15.75">
+    <row r="73" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="2:6">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="8" t="s">
         <v>17</v>
       </c>
@@ -3282,7 +3285,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="2:6">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="9" t="s">
         <v>61</v>
       </c>
@@ -3299,7 +3302,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="76" spans="2:6">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="10" t="s">
         <v>91</v>
       </c>
@@ -3314,7 +3317,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="77" spans="2:6">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="9" t="s">
         <v>92</v>
       </c>
@@ -3329,7 +3332,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="2:6">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="10" t="s">
         <v>93</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="79" spans="2:6">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="9" t="s">
         <v>94</v>
       </c>
@@ -3359,7 +3362,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="2:6">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="9" t="s">
         <v>95</v>
       </c>
@@ -3374,12 +3377,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="84" spans="2:6" ht="15.75">
+    <row r="84" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B84" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="2:6">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="8" t="s">
         <v>17</v>
       </c>
@@ -3396,7 +3399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="2:6">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="9" t="s">
         <v>136</v>
       </c>
@@ -3413,7 +3416,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="2:6">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="10" t="s">
         <v>48</v>
       </c>
@@ -3430,7 +3433,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="2:6">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="9" t="s">
         <v>66</v>
       </c>
@@ -3447,7 +3450,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="2:6">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="10" t="s">
         <v>104</v>
       </c>
@@ -3462,7 +3465,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="90" spans="2:6">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="9" t="s">
         <v>21</v>
       </c>
@@ -3477,7 +3480,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="91" spans="2:6">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" s="9" t="s">
         <v>105</v>
       </c>
@@ -3492,7 +3495,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="95" spans="2:6" ht="15.75">
+    <row r="95" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B95" s="11"/>
     </row>
   </sheetData>
@@ -3524,13 +3527,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.1" customHeight="1">
+    <row r="1" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3538,91 +3541,91 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="61.35" customHeight="1">
+    <row r="2" spans="1:2" ht="61.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="65.099999999999994" customHeight="1">
+    <row r="3" spans="1:2" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="60.6" customHeight="1">
+    <row r="4" spans="1:2" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="59.1" customHeight="1">
+    <row r="5" spans="1:2" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="59.1" customHeight="1">
+    <row r="6" spans="1:2" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="57.6" customHeight="1">
+    <row r="7" spans="1:2" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" ht="57" customHeight="1">
+    <row r="8" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" ht="53.85" customHeight="1">
+    <row r="9" spans="1:2" ht="53.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" ht="53.85" customHeight="1">
+    <row r="10" spans="1:2" ht="53.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" ht="50.85" customHeight="1">
+    <row r="11" spans="1:2" ht="50.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" ht="50.85" customHeight="1">
+    <row r="12" spans="1:2" ht="50.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" ht="47.1" customHeight="1">
+    <row r="13" spans="1:2" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" ht="48" customHeight="1">
+    <row r="14" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" ht="51.6" customHeight="1">
+    <row r="15" spans="1:2" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" ht="50.85" customHeight="1">
+    <row r="16" spans="1:2" ht="50.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>

</xml_diff>